<commit_message>
actualizacion de productos antes del lanzamiento
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3057,10 +3057,8 @@
           <t>Misiones 1242</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>33824565456</t>
-        </is>
+      <c r="D46" t="n">
+        <v>33824565456</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -3099,6 +3097,66 @@
       </c>
       <c r="N46" t="n">
         <v>45</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Veronica</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Misiones 1242</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>33824565456</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2025-02-27</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>16:00 a 19:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Efectivo</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>20520</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Empanadas Congeladas Pollo (12u) (x1)</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>